<commit_message>
correct arm coding for within participant designs
</commit_message>
<xml_diff>
--- a/data/key.xlsx
+++ b/data/key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssu-my.sharepoint.com/personal/5cameb31_solent_ac_uk/Documents/Documents/PhD/Systematic Review/Data Extraction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Dropbox\Research\PhD Students\Current\Bailey\exercise_recovery_modalities_meta\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="412" documentId="8_{511407CD-6716-044F-9580-BC9E29048A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{343BE875-6195-F945-A813-CBAC90CDED28}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A31095-8D1B-4D51-B931-981BE31E4DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="500" windowWidth="22500" windowHeight="15520" xr2:uid="{9BCA5C17-8C5F-0F4E-86BF-A7E8EC5FB0C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{9BCA5C17-8C5F-0F4E-86BF-A7E8EC5FB0C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -857,9 +857,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1203,22 +1202,22 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112:A113"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108:B113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="62.5" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="53.6640625" customWidth="1"/>
-    <col min="7" max="7" width="50.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.875" customWidth="1"/>
+    <col min="5" max="5" width="19.625" customWidth="1"/>
+    <col min="6" max="6" width="53.625" customWidth="1"/>
+    <col min="7" max="7" width="50.375" customWidth="1"/>
     <col min="8" max="8" width="30.5" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1244,7 +1243,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1267,7 +1266,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1290,7 +1289,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1313,7 +1312,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1339,12 +1338,12 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>248</v>
@@ -1362,12 +1361,12 @@
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>248</v>
@@ -1385,7 +1384,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1408,7 +1407,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1431,7 +1430,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1457,12 +1456,12 @@
         <v>256</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>243</v>
@@ -1480,7 +1479,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1503,7 +1502,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1526,7 +1525,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1552,7 +1551,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -1578,7 +1577,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
@@ -1604,7 +1603,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7</v>
       </c>
@@ -1627,7 +1626,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7</v>
       </c>
@@ -1650,7 +1649,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8</v>
       </c>
@@ -1676,12 +1675,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
         <v>43</v>
@@ -1699,12 +1698,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
         <v>43</v>
@@ -1722,7 +1721,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9</v>
       </c>
@@ -1745,7 +1744,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9</v>
       </c>
@@ -1768,7 +1767,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>9</v>
       </c>
@@ -1791,7 +1790,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>9</v>
       </c>
@@ -1814,7 +1813,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>10</v>
       </c>
@@ -1840,7 +1839,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10</v>
       </c>
@@ -1863,7 +1862,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10</v>
       </c>
@@ -1886,7 +1885,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>11</v>
       </c>
@@ -1912,12 +1911,12 @@
         <v>255</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>11</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
         <v>65</v>
@@ -1935,7 +1934,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>12</v>
       </c>
@@ -1961,7 +1960,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>12</v>
       </c>
@@ -1984,7 +1983,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>12</v>
       </c>
@@ -2007,7 +2006,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>13</v>
       </c>
@@ -2030,12 +2029,12 @@
         <v>255</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>13</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
         <v>239</v>
@@ -2053,7 +2052,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>14</v>
       </c>
@@ -2076,7 +2075,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>14</v>
       </c>
@@ -2099,7 +2098,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>15</v>
       </c>
@@ -2122,12 +2121,12 @@
         <v>255</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>15</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" t="s">
         <v>84</v>
@@ -2145,7 +2144,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>16</v>
       </c>
@@ -2168,7 +2167,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>16</v>
       </c>
@@ -2191,7 +2190,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>17</v>
       </c>
@@ -2214,12 +2213,12 @@
         <v>255</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>17</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C43" t="s">
         <v>88</v>
@@ -2237,7 +2236,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>18</v>
       </c>
@@ -2263,12 +2262,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>18</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C45" t="s">
         <v>232</v>
@@ -2286,7 +2285,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>19</v>
       </c>
@@ -2309,7 +2308,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>19</v>
       </c>
@@ -2332,7 +2331,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>20</v>
       </c>
@@ -2355,7 +2354,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>20</v>
       </c>
@@ -2378,7 +2377,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>21</v>
       </c>
@@ -2404,7 +2403,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>21</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>22</v>
       </c>
@@ -2450,7 +2449,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>22</v>
       </c>
@@ -2473,7 +2472,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>22</v>
       </c>
@@ -2496,7 +2495,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>22</v>
       </c>
@@ -2519,7 +2518,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>22</v>
       </c>
@@ -2542,7 +2541,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>23</v>
       </c>
@@ -2565,7 +2564,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>23</v>
       </c>
@@ -2588,7 +2587,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>23</v>
       </c>
@@ -2611,7 +2610,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>24</v>
       </c>
@@ -2637,7 +2636,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>24</v>
       </c>
@@ -2660,7 +2659,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>25</v>
       </c>
@@ -2686,7 +2685,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>25</v>
       </c>
@@ -2709,7 +2708,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>26</v>
       </c>
@@ -2732,12 +2731,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>26</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C65" t="s">
         <v>120</v>
@@ -2755,7 +2754,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>27</v>
       </c>
@@ -2778,7 +2777,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>27</v>
       </c>
@@ -2801,7 +2800,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>27</v>
       </c>
@@ -2824,7 +2823,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>27</v>
       </c>
@@ -2847,7 +2846,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>27</v>
       </c>
@@ -2870,7 +2869,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>28</v>
       </c>
@@ -2896,12 +2895,12 @@
         <v>256</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>28</v>
       </c>
       <c r="B72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C72" t="s">
         <v>133</v>
@@ -2919,7 +2918,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>29</v>
       </c>
@@ -2942,7 +2941,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>29</v>
       </c>
@@ -2965,8 +2964,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="1">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75">
         <v>30</v>
       </c>
       <c r="B75">
@@ -2988,12 +2987,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="1">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76">
         <v>30</v>
       </c>
       <c r="B76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C76" t="s">
         <v>143</v>
@@ -3011,12 +3010,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="1">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77">
         <v>30</v>
       </c>
       <c r="B77">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C77" t="s">
         <v>143</v>
@@ -3034,8 +3033,8 @@
         <v>257</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="1">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78">
         <v>31</v>
       </c>
       <c r="B78">
@@ -3057,12 +3056,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="1">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79">
         <v>31</v>
       </c>
       <c r="B79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C79" t="s">
         <v>148</v>
@@ -3080,8 +3079,8 @@
         <v>257</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="1">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80">
         <v>31</v>
       </c>
       <c r="B80">
@@ -3103,7 +3102,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>32</v>
       </c>
@@ -3126,7 +3125,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>32</v>
       </c>
@@ -3149,7 +3148,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>32</v>
       </c>
@@ -3172,7 +3171,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>33</v>
       </c>
@@ -3195,7 +3194,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>33</v>
       </c>
@@ -3218,7 +3217,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>33</v>
       </c>
@@ -3241,7 +3240,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>33</v>
       </c>
@@ -3264,8 +3263,8 @@
         <v>255</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="1">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88">
         <v>34</v>
       </c>
       <c r="B88">
@@ -3290,12 +3289,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="1">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89">
         <v>34</v>
       </c>
       <c r="B89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C89" t="s">
         <v>164</v>
@@ -3313,12 +3312,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" s="1">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90">
         <v>34</v>
       </c>
       <c r="B90">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C90" t="s">
         <v>164</v>
@@ -3336,7 +3335,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>35</v>
       </c>
@@ -3362,7 +3361,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>35</v>
       </c>
@@ -3385,7 +3384,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>36</v>
       </c>
@@ -3411,7 +3410,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>36</v>
       </c>
@@ -3434,7 +3433,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>36</v>
       </c>
@@ -3457,7 +3456,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>36</v>
       </c>
@@ -3480,7 +3479,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>36</v>
       </c>
@@ -3503,8 +3502,8 @@
         <v>255</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="1">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98">
         <v>37</v>
       </c>
       <c r="B98">
@@ -3529,12 +3528,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="1">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99">
         <v>37</v>
       </c>
       <c r="B99">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C99" t="s">
         <v>183</v>
@@ -3552,8 +3551,8 @@
         <v>257</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="1">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100">
         <v>38</v>
       </c>
       <c r="B100">
@@ -3575,12 +3574,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="1">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101">
         <v>38</v>
       </c>
       <c r="B101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C101" t="s">
         <v>187</v>
@@ -3598,12 +3597,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="1">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102">
         <v>38</v>
       </c>
       <c r="B102">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C102" t="s">
         <v>187</v>
@@ -3621,8 +3620,8 @@
         <v>259</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="1">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103">
         <v>39</v>
       </c>
       <c r="B103">
@@ -3644,12 +3643,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="1">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104">
         <v>39</v>
       </c>
       <c r="B104">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C104" t="s">
         <v>195</v>
@@ -3667,12 +3666,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="1">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105">
         <v>39</v>
       </c>
       <c r="B105">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C105" t="s">
         <v>195</v>
@@ -3690,7 +3689,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>40</v>
       </c>
@@ -3713,7 +3712,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>40</v>
       </c>
@@ -3736,8 +3735,8 @@
         <v>255</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="1">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108">
         <v>41</v>
       </c>
       <c r="B108">
@@ -3762,12 +3761,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="1">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109">
         <v>41</v>
       </c>
       <c r="B109">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C109" t="s">
         <v>203</v>
@@ -3785,12 +3784,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="1">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110">
         <v>41</v>
       </c>
       <c r="B110">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C110" t="s">
         <v>203</v>
@@ -3808,12 +3807,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A111" s="1">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111">
         <v>41</v>
       </c>
       <c r="B111">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C111" t="s">
         <v>203</v>
@@ -3831,8 +3830,8 @@
         <v>257</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="1">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112">
         <v>42</v>
       </c>
       <c r="B112">
@@ -3854,12 +3853,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A113" s="1">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113">
         <v>42</v>
       </c>
       <c r="B113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C113" t="s">
         <v>210</v>
@@ -3877,7 +3876,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>43</v>
       </c>
@@ -3900,7 +3899,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>43</v>
       </c>
@@ -3923,7 +3922,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>44</v>
       </c>
@@ -3946,7 +3945,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>44</v>
       </c>
@@ -3969,7 +3968,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>45</v>
       </c>
@@ -3995,7 +3994,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>45</v>
       </c>
@@ -4018,7 +4017,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>46</v>
       </c>
@@ -4041,7 +4040,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>46</v>
       </c>

</xml_diff>